<commit_message>
updated repo for DD
</commit_message>
<xml_diff>
--- a/paper_links/Presence of properties in articles.xlsx
+++ b/paper_links/Presence of properties in articles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IIT Delhi\Research\papers to study\challenges\Github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IIT Delhi\Research\papers to study\challenges\Identifying_challenges_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>PII</t>
   </si>
@@ -147,12 +147,6 @@
     <t>S0022309303006537</t>
   </si>
   <si>
-    <t>rate eq analysis</t>
-  </si>
-  <si>
-    <t>fig caption</t>
-  </si>
-  <si>
     <t>S0022309304000687</t>
   </si>
   <si>
@@ -238,9 +232,6 @@
   </si>
   <si>
     <t>S0022309309005274</t>
-  </si>
-  <si>
-    <t>structural props</t>
   </si>
 </sst>
 </file>
@@ -739,7 +730,7 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +739,7 @@
     <col min="17" max="17" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -757,45 +748,6 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -831,9 +783,6 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -845,9 +794,6 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -883,9 +829,6 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -897,9 +840,6 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -912,9 +852,6 @@
       <c r="C13">
         <v>1</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -940,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -950,11 +887,8 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -962,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -970,7 +904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -978,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -988,19 +922,10 @@
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1008,14 +933,8 @@
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="L22">
-        <v>1</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1023,240 +942,207 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>43</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>44</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>45</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>48</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>49</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="L30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>50</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>51</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="N32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>52</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>53</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>54</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>55</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>56</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>57</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>59</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="L40">
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>60</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>61</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="L42">
-        <v>1</v>
-      </c>
-      <c r="N42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>62</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>65</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
-      </c>
-      <c r="N47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>67</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1264,7 +1150,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1272,7 +1158,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -1280,7 +1166,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B51">
         <v>1</v>

</xml_diff>